<commit_message>
Fix excel import ncc
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_purchase/static/src/xlsx/banggianhacungcap.xlsx
+++ b/addons/custom/forlife_purchase/static/src/xlsx/banggianhacungcap.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quyetnv30\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aht\Desktop\Forlife\m_onnet_odoo_mfl2201er\addons\custom\forlife_purchase\static\src\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F75782B3-34F5-4B9C-ABDF-41FC4D492B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B194CD40-A6D9-42D6-B1F8-768AE8F1E340}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,15 +44,9 @@
     <t>Biến thể sản phẩm</t>
   </si>
   <si>
-    <t>Số lượng quy đổi</t>
-  </si>
-  <si>
     <t>Số lượng</t>
   </si>
   <si>
-    <t>Đơn vị tính</t>
-  </si>
-  <si>
     <t>Giá</t>
   </si>
   <si>
@@ -97,12 +90,18 @@
   </si>
   <si>
     <t>Đôi</t>
+  </si>
+  <si>
+    <t>Đơn vị mua</t>
+  </si>
+  <si>
+    <t>Tỷ lệ quy đổi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -579,17 +578,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E1EF6C-C828-44EA-A16D-C7639F4C96C3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
@@ -606,39 +609,39 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
@@ -647,13 +650,13 @@
         <v>1</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="I2" s="7">
         <v>45056</v>
@@ -667,13 +670,13 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D3" s="9">
         <v>1</v>
@@ -682,13 +685,13 @@
         <v>1</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I3" s="13">
         <v>45056</v>
@@ -702,13 +705,13 @@
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="9">
         <v>1</v>
@@ -717,13 +720,13 @@
         <v>1</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G4" s="11">
         <v>9</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I4" s="13">
         <v>45056</v>

</xml_diff>